<commit_message>
cleaning up the timing data outout for the main time test
</commit_message>
<xml_diff>
--- a/Data/timings_both_models_2-2_treatments.xlsx
+++ b/Data/timings_both_models_2-2_treatments.xlsx
@@ -16,9 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
   <si>
     <t>model</t>
+  </si>
+  <si>
+    <t>data set</t>
   </si>
   <si>
     <t>T_n</t>
@@ -403,13 +406,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,8 +443,11 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -449,34 +455,37 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.134</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.043</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.039</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>0.042</v>
       </c>
       <c r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L2">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -484,34 +493,37 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>0.052</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>0.041</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>0.038</v>
       </c>
       <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L3">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -519,34 +531,37 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.129</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>0.042</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>0.039</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>0.039</v>
       </c>
       <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L4">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -554,34 +569,37 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>0.042</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>0.044</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>0.044</v>
       </c>
       <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L5">
+        <v>3e-05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -589,34 +607,37 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>0.146</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>0.048</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>0.044</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>0.044</v>
       </c>
       <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L6">
+        <v>3e-05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -624,34 +645,37 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.127</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>0.043</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>0.037</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>0.037</v>
       </c>
       <c r="K7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L7">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -659,34 +683,37 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.123</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>0.038</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>0.037</v>
       </c>
       <c r="K8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L8">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -694,34 +721,37 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>0.147</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>0.047</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>0.046</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>0.045</v>
       </c>
       <c r="K9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L9">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -729,34 +759,37 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>0.136</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>0.046</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>0.042</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>0.038</v>
       </c>
       <c r="K10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L10">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -764,34 +797,37 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>0.126</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>0.041</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>0.038</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>0.038</v>
       </c>
       <c r="K11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L11">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -799,34 +835,37 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.128</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>0.043</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>0.038</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>0.037</v>
       </c>
       <c r="K12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L12">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -834,34 +873,37 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>0.127</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>0.042</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>0.039</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>0.038</v>
       </c>
       <c r="K13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L13">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -869,34 +911,37 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>0.127</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>0.042</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>0.039</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>0.038</v>
       </c>
       <c r="K14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L14">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -904,34 +949,37 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>0.137</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>0.042</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>0.045</v>
       </c>
       <c r="K15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L15">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -939,31 +987,34 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>0.135</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>0.047</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>0.039</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>1000</v>
+      </c>
+      <c r="L16">
+        <v>2e-05</v>
       </c>
     </row>
   </sheetData>
@@ -973,13 +1024,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1010,8 +1061,11 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1019,34 +1073,37 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.259</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.063</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L2">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1054,34 +1111,37 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.258</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>0.063</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>0.063</v>
       </c>
       <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L3">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1089,34 +1149,37 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.26</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L4">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1124,34 +1187,37 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.261</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>0.063</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L5">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1159,34 +1225,37 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>0.26</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L6">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1194,34 +1263,37 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.261</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="K7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L7">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1229,34 +1301,37 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.263</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="K8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L8">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1264,34 +1339,37 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>0.267</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="K9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L9">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1299,34 +1377,37 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>0.264</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="K10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L10">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1334,34 +1415,37 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>0.266</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="K11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L11">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1369,34 +1453,37 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.264</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="K12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L12">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1404,34 +1491,37 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>0.268</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>0.066</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>0.066</v>
       </c>
       <c r="K13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L13">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1439,34 +1529,37 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>0.267</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="K14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L14">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1474,34 +1567,37 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>0.268</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="K15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L15">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1509,31 +1605,34 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>0.268</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>1000</v>
+      </c>
+      <c r="L16">
+        <v>2e-05</v>
       </c>
     </row>
   </sheetData>
@@ -1543,13 +1642,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1580,8 +1679,11 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1589,34 +1691,37 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.134</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.043</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.039</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>0.042</v>
       </c>
       <c r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L2">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1624,34 +1729,37 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>0.052</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>0.041</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>0.038</v>
       </c>
       <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L3">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1659,34 +1767,37 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.129</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>0.042</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>0.039</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>0.039</v>
       </c>
       <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L4">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1694,34 +1805,37 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>0.042</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>0.044</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>0.044</v>
       </c>
       <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L5">
+        <v>3e-05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1729,34 +1843,37 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>0.146</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>0.048</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>0.044</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>0.044</v>
       </c>
       <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L6">
+        <v>3e-05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1764,34 +1881,37 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.127</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>0.043</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>0.037</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>0.037</v>
       </c>
       <c r="K7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L7">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1799,34 +1919,37 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.123</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>0.038</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>0.037</v>
       </c>
       <c r="K8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L8">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1834,34 +1957,37 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>0.147</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>0.047</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>0.046</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>0.045</v>
       </c>
       <c r="K9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L9">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1869,34 +1995,37 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>0.136</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>0.046</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>0.042</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>0.038</v>
       </c>
       <c r="K10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L10">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1904,34 +2033,37 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>0.126</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>0.041</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>0.038</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>0.038</v>
       </c>
       <c r="K11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L11">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1939,34 +2071,37 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.128</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>0.043</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>0.038</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>0.037</v>
       </c>
       <c r="K12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L12">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1974,34 +2109,37 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>0.127</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>0.042</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>0.039</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>0.038</v>
       </c>
       <c r="K13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L13">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2009,34 +2147,37 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>0.127</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>0.042</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>0.039</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>0.038</v>
       </c>
       <c r="K14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L14">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2044,34 +2185,37 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>0.137</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>0.042</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>0.045</v>
       </c>
       <c r="K15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L15">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2079,34 +2223,37 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>0.135</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>0.047</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>0.039</v>
       </c>
       <c r="K16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L16">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="1">
         <v>0</v>
       </c>
@@ -2114,34 +2261,37 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>0.259</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>0.063</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="K17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L17">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -2149,34 +2299,37 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>0.258</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>0.063</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>0.063</v>
       </c>
       <c r="K18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L18">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -2184,34 +2337,37 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>0.26</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="K19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L19">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="1">
         <v>3</v>
       </c>
@@ -2219,34 +2375,37 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>0.261</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>0.063</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="K20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L20">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="1">
         <v>4</v>
       </c>
@@ -2254,34 +2413,37 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>0.26</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="J21">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="K21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L21">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="1">
         <v>5</v>
       </c>
@@ -2289,34 +2451,37 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>0.261</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="K22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L22">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="1">
         <v>6</v>
       </c>
@@ -2324,34 +2489,37 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>0.263</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="K23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L23">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="1">
         <v>7</v>
       </c>
@@ -2359,34 +2527,37 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>0.267</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="K24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L24">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="1">
         <v>8</v>
       </c>
@@ -2394,34 +2565,37 @@
         <v>1</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>0.264</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="K25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L25">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="1">
         <v>9</v>
       </c>
@@ -2429,34 +2603,37 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>0.266</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="K26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L26">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="1">
         <v>10</v>
       </c>
@@ -2464,34 +2641,37 @@
         <v>1</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>0.264</v>
       </c>
       <c r="G27">
         <v>0</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="K27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L27">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="1">
         <v>11</v>
       </c>
@@ -2499,34 +2679,37 @@
         <v>1</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>0.268</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>0.066</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>0.066</v>
       </c>
       <c r="K28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L28">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="1">
         <v>12</v>
       </c>
@@ -2534,34 +2717,37 @@
         <v>1</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>0.267</v>
       </c>
       <c r="G29">
         <v>0</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="J29">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="K29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L29">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="1">
         <v>13</v>
       </c>
@@ -2569,34 +2755,37 @@
         <v>1</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>0.268</v>
       </c>
       <c r="G30">
         <v>0</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="J30">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="K30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
+        <v>1000</v>
+      </c>
+      <c r="L30">
+        <v>2e-05</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="1">
         <v>14</v>
       </c>
@@ -2604,31 +2793,34 @@
         <v>1</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>0.268</v>
       </c>
       <c r="G31">
         <v>0</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="J31">
-        <v>0</v>
+        <v>0.065</v>
       </c>
       <c r="K31">
-        <v>0</v>
+        <v>1000</v>
+      </c>
+      <c r="L31">
+        <v>2e-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>